<commit_message>
Updates to UIAutomation scripts
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/parabank_register.xlsx
+++ b/src/test/java/Resources/parabank_register.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C294887-C4B9-42D0-BC06-3F6B85B5D16E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE61DD-2FEB-4E6C-B3F4-136AED674BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>tcbdemouser</t>
+  </si>
+  <si>
+    <t>tcbdemotestuser2</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +415,7 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
   </cols>
@@ -478,7 +481,7 @@
         <v>1234567890</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updates to Parabank register
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/parabank_register.xlsx
+++ b/src/test/java/Resources/parabank_register.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCE61DD-2FEB-4E6C-B3F4-136AED674BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD04089-0065-48DB-816B-1A39E21B7CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>First Name</t>
   </si>
@@ -73,18 +73,21 @@
     <t>tcbdemouser</t>
   </si>
   <si>
-    <t>tcbdemotestuser2</t>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>tcbdemotestuser11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="00000"/>
-    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
-    <numFmt numFmtId="166" formatCode="000\-00\-0000"/>
-    <numFmt numFmtId="167" formatCode=";;;**"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;**"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -115,12 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +416,7 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
   </cols>
@@ -471,22 +472,22 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1">
-        <v>411057</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>